<commit_message>
Syllable analysis, improvement on spell.txt
</commit_message>
<xml_diff>
--- a/spell-table.xlsx
+++ b/spell-table.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Letter</t>
   </si>
@@ -161,6 +161,18 @@
   </si>
   <si>
     <t>Double Vowels</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>VC</t>
   </si>
 </sst>
 </file>
@@ -887,11 +899,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="313238680"/>
-        <c:axId val="313239072"/>
+        <c:axId val="253094504"/>
+        <c:axId val="253094896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="313238680"/>
+        <c:axId val="253094504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -934,7 +946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313239072"/>
+        <c:crossAx val="253094896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -942,7 +954,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="313239072"/>
+        <c:axId val="253094896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -993,7 +1005,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313238680"/>
+        <c:crossAx val="253094504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1939,10 +1951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,12 +1965,12 @@
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1974,20 +1986,23 @@
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2003,20 +2018,24 @@
       <c r="I2">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" s="1">
+        <f>SUM(G2:I2)</f>
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
         <v>45</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>7</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>10</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2032,20 +2051,24 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J27" si="0">SUM(G3:I3)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
         <v>46</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>5</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>3</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2061,20 +2084,24 @@
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="K4" t="s">
+      <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L4" t="s">
         <v>47</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
       <c r="M4">
         <v>1</v>
       </c>
       <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2090,20 +2117,24 @@
       <c r="I5">
         <v>3</v>
       </c>
-      <c r="K5" t="s">
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L5" t="s">
         <v>48</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2119,8 +2150,15 @@
       <c r="I6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2136,8 +2174,15 @@
       <c r="I7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2153,8 +2198,12 @@
       <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2170,8 +2219,12 @@
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2187,8 +2240,12 @@
       <c r="I10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2204,8 +2261,12 @@
       <c r="I11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2221,8 +2282,12 @@
       <c r="I12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2238,8 +2303,12 @@
       <c r="I13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2255,8 +2324,12 @@
       <c r="I14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>31</v>
       </c>
@@ -2269,8 +2342,12 @@
       <c r="I15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J15" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>32</v>
       </c>
@@ -2283,8 +2360,12 @@
       <c r="I16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>33</v>
       </c>
@@ -2297,8 +2378,12 @@
       <c r="I17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>34</v>
       </c>
@@ -2311,8 +2396,12 @@
       <c r="I18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>35</v>
       </c>
@@ -2325,8 +2414,12 @@
       <c r="I19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>36</v>
       </c>
@@ -2339,8 +2432,12 @@
       <c r="I20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>37</v>
       </c>
@@ -2353,8 +2450,12 @@
       <c r="I21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>38</v>
       </c>
@@ -2367,8 +2468,12 @@
       <c r="I22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>39</v>
       </c>
@@ -2381,8 +2486,12 @@
       <c r="I23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>40</v>
       </c>
@@ -2395,8 +2504,12 @@
       <c r="I24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>41</v>
       </c>
@@ -2409,8 +2522,12 @@
       <c r="I25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>42</v>
       </c>
@@ -2423,8 +2540,12 @@
       <c r="I26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>43</v>
       </c>
@@ -2436,6 +2557,31 @@
       </c>
       <c r="I27">
         <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="1">
+        <f>SUM(G2:G27)</f>
+        <v>30</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" ref="H28:J28" si="1">SUM(H2:H27)</f>
+        <v>30</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J28" s="1">
+        <f>SUM(J2:J27)</f>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented optimal grammar selection
</commit_message>
<xml_diff>
--- a/spell-table.xlsx
+++ b/spell-table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Letter</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>VC</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>CVC</t>
+  </si>
+  <si>
+    <t>CCV</t>
   </si>
 </sst>
 </file>
@@ -899,11 +908,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="253094504"/>
-        <c:axId val="253094896"/>
+        <c:axId val="271821328"/>
+        <c:axId val="271819760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="253094504"/>
+        <c:axId val="271821328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,7 +955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253094896"/>
+        <c:crossAx val="271819760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -954,7 +963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253094896"/>
+        <c:axId val="271819760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1005,7 +1014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253094504"/>
+        <c:crossAx val="271821328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1953,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2155,7 +2164,16 @@
         <v>9</v>
       </c>
       <c r="L6" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2179,7 +2197,16 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2202,6 +2229,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L8" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2223,6 +2262,18 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="L9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2244,6 +2295,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="L10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2265,6 +2328,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2572,7 +2647,7 @@
         <v>30</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" ref="H28:J28" si="1">SUM(H2:H27)</f>
+        <f t="shared" ref="H28:I28" si="1">SUM(H2:H27)</f>
         <v>30</v>
       </c>
       <c r="I28" s="1">

</xml_diff>